<commit_message>
Add intrarow and tokens in column names
</commit_message>
<xml_diff>
--- a/tests/data/surveys.xlsx
+++ b/tests/data/surveys.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\excelextract\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B130291-08A0-4773-99C9-0D41783EE609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAEC0FED-A01A-4777-819A-475C3FBB50A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="overview" sheetId="1" r:id="rId1"/>
     <sheet name="company 1" sheetId="2" r:id="rId2"/>
     <sheet name="company 2" sheetId="3" r:id="rId3"/>
+    <sheet name="basic" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="27">
   <si>
     <t>Name</t>
   </si>
@@ -428,7 +429,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -469,7 +470,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection sqref="A1:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,4 +914,134 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D277EADB-9B6D-489D-8369-93B9111DD396}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>30000</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>40000</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>60000</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>50000</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add auto type detection and more types
</commit_message>
<xml_diff>
--- a/tests/data/surveys.xlsx
+++ b/tests/data/surveys.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\excelextract\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAEC0FED-A01A-4777-819A-475C3FBB50A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D9178D-4657-4676-ACB8-81DFC7DC6399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="overview" sheetId="1" r:id="rId1"/>
     <sheet name="company 1" sheetId="2" r:id="rId2"/>
     <sheet name="company 2" sheetId="3" r:id="rId3"/>
     <sheet name="basic" sheetId="4" r:id="rId4"/>
+    <sheet name="types" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="41">
   <si>
     <t>Name</t>
   </si>
@@ -109,12 +110,57 @@
   </si>
   <si>
     <t>FindCellTest</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>2025-05-05</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>percentage</t>
+  </si>
+  <si>
+    <t>scientific</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>17h00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -144,9 +190,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -920,7 +971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D277EADB-9B6D-489D-8369-93B9111DD396}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -1044,4 +1095,160 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25F44035-8862-46CE-9D0B-A37733A832C5}">
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="24.5703125" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45782</v>
+      </c>
+      <c r="C2" s="1">
+        <v>45782.625</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="3">
+        <v>5</v>
+      </c>
+      <c r="I2" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="J2" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>45782</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="1">
+        <v>45782</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>10</v>
+      </c>
+      <c r="I3">
+        <v>0.1</v>
+      </c>
+      <c r="J3" s="5">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2.4</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>4.5</v>
+      </c>
+      <c r="I4">
+        <v>50</v>
+      </c>
+      <c r="J4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5">
+        <v>0.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>